<commit_message>
edit ICD, Database funcs
</commit_message>
<xml_diff>
--- a/IWAS/workingsheet.xlsx
+++ b/IWAS/workingsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="113">
   <si>
     <t>registData</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -225,26 +225,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>보고</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>우선순위변경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>담당자변경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일정변경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제목변경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>진척도</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -272,10 +252,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pri</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -329,10 +305,6 @@
   </si>
   <si>
     <t>chatID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -399,26 +371,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[title]B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[worker]user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[priority]urgent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[due]180506</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[status]message</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>VARCHAR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -496,6 +448,30 @@
   </si>
   <si>
     <t>state</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UINT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>worker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>message</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>urgent</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -849,7 +825,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -863,35 +839,35 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -919,7 +895,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -936,140 +912,140 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="Q1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" t="s">
+      <c r="R1" t="s">
         <v>71</v>
-      </c>
-      <c r="L1" t="s">
-        <v>72</v>
-      </c>
-      <c r="M1" t="s">
-        <v>74</v>
-      </c>
-      <c r="N1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O1" t="s">
-        <v>118</v>
-      </c>
-      <c r="P1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>76</v>
-      </c>
-      <c r="R1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="O2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P2" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="Q2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="R2" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="49.5">
       <c r="A3" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
         <v>81</v>
       </c>
-      <c r="C3" t="s">
-        <v>88</v>
-      </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="J3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="K3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -1080,7 +1056,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1119,7 +1095,7 @@
         <v>14</v>
       </c>
       <c r="P4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="Q4" t="s">
         <v>30</v>
@@ -1136,7 +1112,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -1159,7 +1135,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I6" t="s">
         <v>28</v>
@@ -1173,7 +1149,7 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1208,7 +1184,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1224,62 +1200,62 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
         <v>85</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="49.5">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
         <v>81</v>
-      </c>
-      <c r="C3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1293,53 +1269,53 @@
         <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="C5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="C6" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="F6" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="C7" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="C8" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="C9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" t="s">
-        <v>97</v>
+        <v>67</v>
+      </c>
+      <c r="F9">
+        <v>180506</v>
       </c>
     </row>
   </sheetData>
@@ -1353,7 +1329,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1365,56 +1341,56 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="49.5">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1445,7 +1421,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:F10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1461,64 +1437,64 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="49.5">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -1527,7 +1503,7 @@
         <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
         <v>33</v>
@@ -1541,16 +1517,16 @@
         <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
       <c r="C6" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F6" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -1559,7 +1535,7 @@
         <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1567,7 +1543,7 @@
         <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1575,7 +1551,7 @@
         <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1583,15 +1559,15 @@
         <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="C11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update chat system on server
</commit_message>
<xml_diff>
--- a/IWAS/workingsheet.xlsx
+++ b/IWAS/workingsheet.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="24735" windowHeight="12060" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="24735" windowHeight="12060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
     <sheet name="task" sheetId="2" r:id="rId2"/>
     <sheet name="taskHistory" sheetId="6" r:id="rId3"/>
     <sheet name="chat" sheetId="4" r:id="rId4"/>
-    <sheet name="charHistory" sheetId="3" r:id="rId5"/>
+    <sheet name="chatHistory" sheetId="3" r:id="rId5"/>
     <sheet name="file" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
   <si>
     <t>registData</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -137,10 +137,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>메세지전송</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>전송자</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -174,26 +170,6 @@
   </si>
   <si>
     <t>파일이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동작 타입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>접속자추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>접속자제거</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>파일업로드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>파일다운로드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -308,10 +284,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>command</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>변경 내용</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -324,10 +296,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>taskIDs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>전송시간</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -408,31 +376,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Task 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Task 삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>message</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>taskID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fileID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>채팅방 생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -800,44 +744,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -883,128 +827,128 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="N1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="R1" t="s">
         <v>52</v>
-      </c>
-      <c r="J1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" t="s">
-        <v>92</v>
-      </c>
-      <c r="L1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O1" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>56</v>
-      </c>
-      <c r="R1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="I2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="J2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="K2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="L2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="M2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="N2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="O2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="P2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="Q2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="R2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="49.5">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -1015,7 +959,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1042,13 +986,13 @@
         <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="M4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="N4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="O4" t="s">
         <v>12</v>
@@ -1057,7 +1001,7 @@
         <v>27</v>
       </c>
       <c r="Q4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="R4" t="s">
         <v>15</v>
@@ -1071,7 +1015,7 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
         <v>18</v>
@@ -1094,7 +1038,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I6" t="s">
         <v>26</v>
@@ -1108,7 +1052,7 @@
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1159,90 +1103,90 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="E5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="E6" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="E7" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="E8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1253,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1264,66 +1208,60 @@
     <col min="1" max="6" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="49.5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -1340,161 +1278,93 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
-    <col min="3" max="4" width="14.75" customWidth="1"/>
-    <col min="5" max="5" width="11.75" customWidth="1"/>
-    <col min="6" max="6" width="22.5" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
-    <col min="9" max="9" width="15.5" customWidth="1"/>
-    <col min="11" max="11" width="17.25" customWidth="1"/>
+    <col min="3" max="3" width="14.75" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="49.5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="49.5">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>98</v>
-      </c>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="C8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="C10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="C11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="C12" t="s">
-        <v>102</v>
-      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1519,25 +1389,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>37</v>
-      </c>
-      <c r="G1" t="s">
-        <v>38</v>
       </c>
       <c r="H1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
fixed user column name issue
</commit_message>
<xml_diff>
--- a/IWAS/workingsheet.xlsx
+++ b/IWAS/workingsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="24735" windowHeight="12060" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="24735" windowHeight="12060"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="100">
   <si>
     <t>registData</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -377,6 +377,50 @@
   </si>
   <si>
     <t>message</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>not null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메시지 종류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메시지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>password</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -729,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -747,7 +791,7 @@
         <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
@@ -1199,7 +1243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1278,24 +1322,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
     <col min="3" max="3" width="14.75" customWidth="1"/>
-    <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="5" max="5" width="22.5" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="17.25" customWidth="1"/>
+    <col min="4" max="5" width="11.75" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -1309,10 +1353,13 @@
         <v>62</v>
       </c>
       <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -1326,10 +1373,13 @@
         <v>86</v>
       </c>
       <c r="E2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="49.5">
+    <row r="3" spans="1:11" ht="49.5">
       <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
@@ -1342,8 +1392,11 @@
       <c r="D3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -1357,14 +1410,44 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="E5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="E7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
change time type to long
</commit_message>
<xml_diff>
--- a/IWAS/workingsheet.xlsx
+++ b/IWAS/workingsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="14385" windowHeight="12060" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="14385" windowHeight="12060"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="116">
   <si>
     <t>registData</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -481,6 +481,10 @@
   </si>
   <si>
     <t>"confirmNO"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BIGINT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -856,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -891,7 +895,7 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
         <v>74</v>
@@ -935,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1025,7 +1029,7 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
         <v>80</v>
@@ -1052,13 +1056,13 @@
         <v>80</v>
       </c>
       <c r="L2" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="M2" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="N2" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="O2" t="s">
         <v>80</v>
@@ -1072,11 +1076,11 @@
       <c r="R2" t="s">
         <v>74</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>80</v>
+      <c r="S2" t="s">
+        <v>115</v>
+      </c>
+      <c r="T2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="49.5">
@@ -1092,8 +1096,6 @@
       <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
@@ -1182,8 +1184,6 @@
       <c r="O5" t="s">
         <v>107</v>
       </c>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6">
@@ -1250,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1297,7 +1297,7 @@
         <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
         <v>80</v>
@@ -1380,7 +1380,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1407,7 +1407,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
         <v>80</v>
@@ -1455,7 +1455,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1497,7 +1497,7 @@
         <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
         <v>80</v>
@@ -1606,7 +1606,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>